<commit_message>
Testing method for the ATE functionality
</commit_message>
<xml_diff>
--- a/testing/communitySmellsDataset.xlsx
+++ b/testing/communitySmellsDataset.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
@@ -5222,6 +5222,2576 @@
         </is>
       </c>
     </row>
+    <row r="65">
+      <c r="A65" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="3" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="3" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="3" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="3" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="3" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="3" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="3" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="3" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="3" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="3" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="3" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="3" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="3" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="3" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="3" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="3" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="3" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="3" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="3" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="3" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="3" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="3" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="3" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O89" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="3" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="3" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="3" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="3" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="3" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O94" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="3" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O95" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="3" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="3" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>24/05/2022 00:26:00</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O97" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="3" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>https://github.com/test/testRepository</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>testRepository</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="O98" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="3" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>https://github.com/tensorflow/ranking</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>ranking</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>tensorflow</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>12/03/2018</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="O99" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>